<commit_message>
Standardize UI layout with ListPage, DataTable, FilterBar, and GroupBy components
Adds reusable ListPage, DataTable, FilterBar, and GroupBy components for
consistent page layouts. Migrates all list pages (employees, leave, roles,
users, training courses, onboarding items, employee statuses, audit log,
my training) to use these shared components. Fixes settings page button
placement, adds self-service training status endpoint, and unifies search
placeholder text.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/work/changelog.xlsx
+++ b/work/changelog.xlsx
@@ -15,10 +15,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
     <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -49,11 +50,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -887,6 +889,56 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>46060</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0.5.4</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>ListPage component with built-in search and FilterBar toolbar. Standardised filtering across all pages using FilterBar (replaces standalone Select dropdowns). Migrated training courses page. Documented UI layout conventions (work/ui-layout/).</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="n">
+        <v>46060</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0.5.5</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>DataTable component for tabular records (flat or expandable rows). Merged notifications into audit log page as tab. Migrated all list pages to ListPage+ListRow+FilterBar: employees, users, my-training, leave, onboarding items, employee statuses. Updated employee-leave-tab to use ListRow.</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Archive appraisals-rework and ui-layout work directories, update changelog
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/work/changelog.xlsx
+++ b/work/changelog.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -939,6 +939,106 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>46060</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0.5.6</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Appraisals rework: replaced matrix view with DataGrid-based grid showing appraisal status by year. Added modal for scheduling, completing, and editing appraisals with notes and outcome fields.</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>46060</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0.5.7</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Enhancement</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Migrated roles page to ListPage+ListRow. Added search to roles, onboarding items, and employee statuses. Fixed DataTable header text inconsistency. Fixed settings page tab padding and consolidated Save buttons with SaveBar component.</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>46060</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0.5.8</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>GroupBy component for dynamic list grouping. Added to My Training page with Category/Status options. CollapsibleSection now supports controlled mode. ListPage has expand/collapse all toggle icon.</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>46060</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0.5.9</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Training status endpoint self-service fallback: users without training_matrix.view permission can now see their own training status. Fixed My Training RecordTrainingModal not rendering when groups active.</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Microsoft Entra ID SSO with JIT provisioning and employee auto-matching
- Switch MSAL from loginPopup to loginRedirect for reliable auth flow
- Add auth_method column (password/microsoft/both) to users model
- Make password_hash nullable for microsoft-only users
- JIT-create users with Employee role on first Microsoft login
- Auto-match employee records by email on Microsoft login
- Add auth method controls to Users management page
- Fix StrictMode double-init with ref guard in auth context
- Fix Supabase DB password after reset (propagation delay issue)
- Status: core flow working, further testing needed

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/work/changelog.xlsx
+++ b/work/changelog.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1039,6 +1039,56 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
+        <v>46061</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0.6.0</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Dashboard enhancement: expanded company dashboard (4 stat cards with links, unified alerts merging training/supervision/appraisals, activity feed from audit log). Redesigned personal dashboard (scheduled vs contracted hours chart with month selector, training pie with category dropdown, clickable charts navigating to filtered pages, supervision next-due date, upcoming shifts panel). Shared libs: shift-colors, audit-messages, activity-feed, upcoming-shifts, formatRelativeTime. Backend: self-service rota fallback in RotaController. URL param filtering for my-training and my-rota. Clean chart re-render keys across all graphs.</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="n">
+        <v>46061</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0.7.0</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Microsoft Entra ID SSO: MSAL redirect login flow, JIT user provisioning with Employee role, auto-match employees by email, auth_method column (password/microsoft/both), nullable password_hash, Users page auth method controls. Status: core flow working, further testing needed.</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update changelog with February 2026 entries
Added 7 changelog entries covering:
- Feb 9: Voice capture, mobile scrolling fix, error handling
- Feb 8: AI Providers UI reorganization, ai_providers table architecture, Day in the Life feature
- Feb 7: Dashboard enhancements

Changelog now at 33 rows (was 26).

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/work/changelog.xlsx
+++ b/work/changelog.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1089,6 +1089,195 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-02-09</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Voice Capture: Added push-to-talk voice input for Day in the Life with real-time transcript preview (Web Speech API)</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-02-09</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Bug Fix</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Dashboard Mobile Scrolling: Fixed scrolling issues on mobile devices by removing height constraints</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-02-09</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Bug Fix</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Day in the Life Error Handling: Fixed streaming issues (infinite thinking, send button not activating, SSE error parsing)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>UI Enhancement</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>AI Providers UI: Moved AI Providers management into Settings as tab with ListRow component for compact display</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>AI Providers Architecture: Implemented ai_providers table with CRUD operations, multi-provider support, real-time model fetching from Gemini/Anthropic/OpenAI APIs</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-02-08</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Day in the Life: AI-powered chat interface for generating PACE-informed care observations. Supports Anthropic (Claude), OpenAI (GPT), Gemini with SSE streaming and custom prompts</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Dashboard Enhancements: Enhanced company/personal dashboards with comprehensive data visibility, activity feeds, upcoming shifts, tabbed detail views for all features</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Claude</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>